<commit_message>
add testCase and new python test files
</commit_message>
<xml_diff>
--- a/docs/MeshSr_OFTest.xlsx
+++ b/docs/MeshSr_OFTest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.103\Coding\MeshSr_OFTest\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.102\Coding\MeshSr_OFTest\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="236">
   <si>
     <t>Class Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -968,12 +968,127 @@
     <t>actions.SequentialExecution</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>TEST SUITE 80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestCase 80.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestCase 80.20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestCase 80.30</t>
+  </si>
+  <si>
+    <t>TestCase 80.40</t>
+  </si>
+  <si>
+    <t>TestCase 80.50</t>
+  </si>
+  <si>
+    <t>TestCase 80.60</t>
+  </si>
+  <si>
+    <t>TestCase 80.70</t>
+  </si>
+  <si>
+    <t>TestCase 80.80</t>
+  </si>
+  <si>
+    <t>TestCase 80.90</t>
+  </si>
+  <si>
+    <t>TestCase 80.100</t>
+  </si>
+  <si>
+    <t>TestCase 80.110</t>
+  </si>
+  <si>
+    <t>TestCase 80.120</t>
+  </si>
+  <si>
+    <t>TestCase 80.130</t>
+  </si>
+  <si>
+    <t>TestCase 80.140</t>
+  </si>
+  <si>
+    <t>TestCase 80.150</t>
+  </si>
+  <si>
+    <t>TestCase 80.160</t>
+  </si>
+  <si>
+    <t>1.3 not support</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestCase 80.170</t>
+  </si>
+  <si>
+    <t>TestCase 80.180</t>
+  </si>
+  <si>
+    <t>TestCase 80.190</t>
+  </si>
+  <si>
+    <t>TestCase 80.200</t>
+  </si>
+  <si>
+    <t>TestCase 80.210</t>
+  </si>
+  <si>
+    <t>TestCase 80.220</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">verify the handling of fragments is consistent with the returned configuration </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>???????</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestCase 80.230</t>
+  </si>
+  <si>
+    <t>TestCase 80.240</t>
+  </si>
+  <si>
+    <t>TestCase 80.250</t>
+  </si>
+  <si>
+    <t>TestCase 80.260</t>
+  </si>
+  <si>
+    <t>TestCase 80.270</t>
+  </si>
+  <si>
+    <t>TestCase 80.280</t>
+  </si>
+  <si>
+    <t>TestCase 80.290</t>
+  </si>
+  <si>
+    <t>TestCase 80.300</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1013,6 +1128,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -1374,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -1385,7 +1506,7 @@
     <col min="1" max="1" width="28.75" style="5" customWidth="1"/>
     <col min="2" max="2" width="36.25" style="2" customWidth="1"/>
     <col min="3" max="3" width="9" style="2"/>
-    <col min="4" max="4" width="11.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="60.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="87.375" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
@@ -2389,6 +2510,191 @@
         <v>200</v>
       </c>
     </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A108" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A109" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A110" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A111" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A112" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A113" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A114" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A115" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A116" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A117" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A118" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A119" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A120" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A121" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A122" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A123" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A124" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A125" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A126" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A127" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A128" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A129" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A130" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A131" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A132" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A133" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A134" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A135" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A136" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A137" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A138" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>